<commit_message>
Updates and initial trial of Gurobi Optimizer
</commit_message>
<xml_diff>
--- a/Initial_Usage_List.xlsx
+++ b/Initial_Usage_List.xlsx
@@ -478,25 +478,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2482</v>
+        <v>0.3652</v>
       </c>
       <c r="C2" t="n">
-        <v>0.42</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1747</v>
+        <v>0.1939</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3294</v>
+        <v>0.3794000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>0.39876</v>
+        <v>0.56296</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2882</v>
+        <v>0.2232</v>
       </c>
       <c r="H2" t="n">
-        <v>0.178</v>
+        <v>0.2518</v>
       </c>
     </row>
     <row r="3">
@@ -506,25 +506,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2482</v>
+        <v>0.3452</v>
       </c>
       <c r="C3" t="n">
-        <v>0.42</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2787</v>
+        <v>0.2979</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3294</v>
+        <v>0.3794000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>0.29476</v>
+        <v>0.45896</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2882</v>
+        <v>0.2432</v>
       </c>
       <c r="H3" t="n">
-        <v>0.178</v>
+        <v>0.2518</v>
       </c>
     </row>
     <row r="4">
@@ -534,25 +534,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2482</v>
+        <v>0.3452</v>
       </c>
       <c r="C4" t="n">
-        <v>0.42</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2787</v>
+        <v>0.2979</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3294</v>
+        <v>0.3794000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>0.29476</v>
+        <v>0.4789600000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2882</v>
+        <v>0.2232</v>
       </c>
       <c r="H4" t="n">
-        <v>0.178</v>
+        <v>0.2518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>